<commit_message>
Organização Repositório (algumas apresentações e planilhas)
</commit_message>
<xml_diff>
--- a/Apresentacoes/DiagramasRank.xlsx
+++ b/Apresentacoes/DiagramasRank.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1c419c70cd142ba6/0-Atuais/1-Carreira_Academica/0-INPE/CSBC_artigo/tabela/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_8D5D7F98480054086C0C625CFAE9E5EF39359624" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{31773B87-9385-4BD7-BBE2-22157425D81E}"/>
   <bookViews>
-    <workbookView windowWidth="19665" windowHeight="7980" activeTab="3"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="10845" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,7 +18,18 @@
     <sheet name="tabelona" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -669,17 +686,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="7">
-    <numFmt numFmtId="176" formatCode="0.0E+00"/>
-    <numFmt numFmtId="177" formatCode="0.000E+00"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="0.0000E+00"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="0.0E+00"/>
+    <numFmt numFmtId="165" formatCode="0.000E+00"/>
+    <numFmt numFmtId="168" formatCode="0.0000E+00"/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -728,152 +741,8 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="34">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -882,198 +751,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.15"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -1083,16 +766,16 @@
     </border>
     <border>
       <left style="thin">
-        <color auto="true"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color auto="true"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color auto="true"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color auto="true"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1133,7 +816,7 @@
         <color theme="0"/>
       </top>
       <bottom style="thin">
-        <color auto="true"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1144,7 +827,7 @@
         <color theme="0"/>
       </top>
       <bottom style="thin">
-        <color auto="true"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1155,7 +838,7 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color auto="true"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1164,7 +847,7 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color auto="true"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1177,7 +860,7 @@
         <color theme="0"/>
       </top>
       <bottom style="thin">
-        <color auto="true"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1188,7 +871,7 @@
       </right>
       <top/>
       <bottom style="thin">
-        <color auto="true"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1201,493 +884,213 @@
       </right>
       <top/>
       <bottom style="thin">
-        <color auto="true"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="15" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="18" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="13" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="13" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="11" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true" applyBorder="true">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true" applyBorder="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
-    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
-    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
-    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
-    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
-    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
-    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
-    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
-    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
-    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
-    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
-    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
-    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
-    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
-    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
-    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
-    <cellStyle name="Total" xfId="25" builtinId="25"/>
-    <cellStyle name="Output" xfId="26" builtinId="21"/>
-    <cellStyle name="Currency" xfId="27" builtinId="4"/>
-    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
-    <cellStyle name="Note" xfId="29" builtinId="10"/>
-    <cellStyle name="Input" xfId="30" builtinId="20"/>
-    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
-    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
-    <cellStyle name="Good" xfId="33" builtinId="26"/>
-    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
-    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
-    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
-    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
-    <cellStyle name="Title" xfId="39" builtinId="15"/>
-    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
-    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
-    <cellStyle name="Comma" xfId="44" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
-    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
-    <cellStyle name="Percent" xfId="47" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="false"/>
-  <c:lang val="zh-CN"/>
-  <c:roundedCorners val="false"/>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
       <c14:style val="102"/>
@@ -1697,12 +1100,12 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="true"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
-        <c:varyColors val="false"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1729,9 +1132,6 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:dLbls>
-            <c:delete val="true"/>
-          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>Sheet2!$C$2:$G$2</c:f>
@@ -1779,7 +1179,12 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="false"/>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F64F-41CD-B123-FDC19CBCE9B3}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -1807,9 +1212,6 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:dLbls>
-            <c:delete val="true"/>
-          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>Sheet2!$C$2:$G$2</c:f>
@@ -1857,7 +1259,12 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="false"/>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F64F-41CD-B123-FDC19CBCE9B3}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -1885,9 +1292,6 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:dLbls>
-            <c:delete val="true"/>
-          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>Sheet2!$C$2:$G$2</c:f>
@@ -1935,7 +1339,12 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="false"/>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-F64F-41CD-B123-FDC19CBCE9B3}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1963,9 +1372,6 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:dLbls>
-            <c:delete val="true"/>
-          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>Sheet2!$C$2:$G$2</c:f>
@@ -2013,7 +1419,12 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="false"/>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-F64F-41CD-B123-FDC19CBCE9B3}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
@@ -2041,9 +1452,6 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:dLbls>
-            <c:delete val="true"/>
-          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>Sheet2!$C$2:$G$2</c:f>
@@ -2091,7 +1499,12 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="false"/>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-F64F-41CD-B123-FDC19CBCE9B3}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="5"/>
@@ -2119,9 +1532,6 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:dLbls>
-            <c:delete val="true"/>
-          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>Sheet2!$C$2:$G$2</c:f>
@@ -2169,18 +1579,22 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="false"/>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-F64F-41CD-B123-FDC19CBCE9B3}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:showLegendKey val="false"/>
-          <c:showVal val="false"/>
-          <c:showCatName val="false"/>
-          <c:showSerName val="false"/>
-          <c:showPercent val="false"/>
-          <c:showBubbleSize val="false"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="false"/>
-        <c:smooth val="false"/>
+        <c:smooth val="0"/>
         <c:axId val="619722454"/>
         <c:axId val="858238197"/>
       </c:lineChart>
@@ -2189,8 +1603,9 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="false"/>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2205,7 +1620,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="true"/>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -2218,14 +1633,15 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="858238197"/>
         <c:crosses val="max"/>
-        <c:auto val="false"/>
+        <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="false"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="858238197"/>
@@ -2234,7 +1650,7 @@
           <c:max val="6"/>
           <c:min val="1"/>
         </c:scaling>
-        <c:delete val="false"/>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -2250,7 +1666,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="true"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2264,7 +1680,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="true"/>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -2277,6 +1693,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="619722454"/>
@@ -2295,8 +1712,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
-      <c:overlay val="false"/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -2305,7 +1721,7 @@
         <a:effectLst/>
       </c:spPr>
       <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="true"/>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
         <a:lstStyle/>
         <a:p>
           <a:pPr>
@@ -2321,12 +1737,13 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
         </a:p>
       </c:txPr>
     </c:legend>
-    <c:plotVisOnly val="true"/>
+    <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="false"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2350,6 +1767,7 @@
       <a:pPr>
         <a:defRPr lang="en-US"/>
       </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2496,7 +1914,7 @@
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="true">
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
       <a:spAutoFit/>
     </cs:bodyPr>
   </cs:dataLabelCallout>
@@ -2917,7 +2335,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
@@ -2931,14 +2349,20 @@
       <xdr:row>16</xdr:row>
       <xdr:rowOff>79375</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5734050" y="231775"/>
-        <a:ext cx="4572000" cy="2743200"/>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3069,7 +2493,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="true">
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -3093,9 +2517,9 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="false"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="true">
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -3119,7 +2543,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="false"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -3172,7 +2596,7 @@
             <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill rotWithShape="true">
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -3197,736 +2621,732 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="false"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:K22"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" topLeftCell="B5" workbookViewId="0">
+    <sheetView topLeftCell="B5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="13.375" customWidth="true"/>
-    <col min="3" max="3" width="55.125" customWidth="true"/>
-    <col min="4" max="4" width="10.25" customWidth="true"/>
-    <col min="5" max="5" width="10.625" customWidth="true"/>
-    <col min="6" max="6" width="11.5" customWidth="true"/>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
+    <col min="3" max="3" width="55.140625" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11">
-      <c r="B2" s="50" t="s">
+    <row r="2" spans="1:11">
+      <c r="B2" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="50" t="s">
+      <c r="C2" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="50" t="s">
+      <c r="D2" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="50" t="s">
+      <c r="E2" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="50" t="s">
+      <c r="F2" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="50" t="s">
+      <c r="G2" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="50" t="s">
+      <c r="H2" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="55" t="s">
+      <c r="I2" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="55" t="s">
+      <c r="J2" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="55" t="s">
+      <c r="K2" s="50" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" ht="37" customHeight="true" spans="2:11">
-      <c r="B3" s="51" t="s">
+    <row r="3" spans="1:11" ht="36.950000000000003" customHeight="1">
+      <c r="B3" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="52" t="s">
+      <c r="C3" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="51">
+      <c r="D3" s="46">
         <v>7</v>
       </c>
-      <c r="E3" s="51">
+      <c r="E3" s="46">
         <v>9</v>
       </c>
-      <c r="F3" s="51">
+      <c r="F3" s="46">
         <v>9</v>
       </c>
-      <c r="G3" s="51">
+      <c r="G3" s="46">
         <v>6</v>
       </c>
-      <c r="H3" s="51">
+      <c r="H3" s="46">
         <v>7</v>
       </c>
-      <c r="I3" s="55">
+      <c r="I3" s="50">
         <f>AVERAGE(D3:H3)</f>
         <v>7.6</v>
       </c>
-      <c r="J3" s="55">
+      <c r="J3" s="50">
         <f>MEDIAN(D3:H3)</f>
         <v>7</v>
       </c>
-      <c r="K3" s="55">
+      <c r="K3" s="50">
         <f>MODE(D3:H3)</f>
         <v>7</v>
       </c>
     </row>
-    <row r="4" ht="38" customHeight="true" spans="2:11">
-      <c r="B4" s="51" t="s">
+    <row r="4" spans="1:11" ht="38.1" customHeight="1">
+      <c r="B4" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="52" t="s">
+      <c r="C4" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="51">
+      <c r="D4" s="46">
         <v>4</v>
       </c>
-      <c r="E4" s="51">
+      <c r="E4" s="46">
         <v>4</v>
       </c>
-      <c r="F4" s="51">
+      <c r="F4" s="46">
         <v>4</v>
       </c>
-      <c r="G4" s="51">
+      <c r="G4" s="46">
         <v>2</v>
       </c>
-      <c r="H4" s="51">
+      <c r="H4" s="46">
         <v>3</v>
       </c>
-      <c r="I4" s="55">
+      <c r="I4" s="50">
         <f t="shared" ref="I4:I11" si="0">AVERAGE(D4:H4)</f>
         <v>3.4</v>
       </c>
-      <c r="J4" s="55">
+      <c r="J4" s="50">
         <f t="shared" ref="J4:J11" si="1">MEDIAN(D4:H4)</f>
         <v>4</v>
       </c>
-      <c r="K4" s="55">
+      <c r="K4" s="50">
         <f t="shared" ref="K4:K11" si="2">MODE(D4:H4)</f>
         <v>4</v>
       </c>
     </row>
-    <row r="5" ht="42.75" spans="2:11">
-      <c r="B5" s="51" t="s">
+    <row r="5" spans="1:11" ht="45">
+      <c r="B5" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="52" t="s">
+      <c r="C5" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="51">
+      <c r="D5" s="46">
         <v>8</v>
       </c>
-      <c r="E5" s="51">
+      <c r="E5" s="46">
         <v>8</v>
       </c>
-      <c r="F5" s="51">
+      <c r="F5" s="46">
         <v>8</v>
       </c>
-      <c r="G5" s="51">
+      <c r="G5" s="46">
         <v>5</v>
       </c>
-      <c r="H5" s="51">
+      <c r="H5" s="46">
         <v>9</v>
       </c>
-      <c r="I5" s="55">
+      <c r="I5" s="50">
         <f t="shared" si="0"/>
         <v>7.6</v>
       </c>
-      <c r="J5" s="55">
+      <c r="J5" s="50">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="K5" s="55">
+      <c r="K5" s="50">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
     </row>
-    <row r="6" ht="42.75" spans="2:11">
-      <c r="B6" s="51" t="s">
+    <row r="6" spans="1:11" ht="45">
+      <c r="B6" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="52" t="s">
+      <c r="C6" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="51">
+      <c r="D6" s="46">
         <v>6</v>
       </c>
-      <c r="E6" s="51">
+      <c r="E6" s="46">
         <v>6</v>
       </c>
-      <c r="F6" s="51">
+      <c r="F6" s="46">
         <v>6</v>
       </c>
-      <c r="G6" s="51">
+      <c r="G6" s="46">
         <v>3</v>
       </c>
-      <c r="H6" s="51">
+      <c r="H6" s="46">
         <v>8</v>
       </c>
-      <c r="I6" s="55">
+      <c r="I6" s="50">
         <f t="shared" si="0"/>
         <v>5.8</v>
       </c>
-      <c r="J6" s="55">
+      <c r="J6" s="50">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="K6" s="55">
+      <c r="K6" s="50">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
     </row>
-    <row r="7" ht="42.75" spans="2:11">
-      <c r="B7" s="51" t="s">
+    <row r="7" spans="1:11" ht="45">
+      <c r="B7" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="52" t="s">
+      <c r="C7" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="51">
+      <c r="D7" s="46">
         <v>9</v>
       </c>
-      <c r="E7" s="51">
+      <c r="E7" s="46">
         <v>7</v>
       </c>
-      <c r="F7" s="51">
+      <c r="F7" s="46">
         <v>7</v>
       </c>
-      <c r="G7" s="51">
+      <c r="G7" s="46">
         <v>4</v>
       </c>
-      <c r="H7" s="51">
+      <c r="H7" s="46">
         <v>6</v>
       </c>
-      <c r="I7" s="55">
+      <c r="I7" s="50">
         <f t="shared" si="0"/>
         <v>6.6</v>
       </c>
-      <c r="J7" s="55">
+      <c r="J7" s="50">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="K7" s="55">
+      <c r="K7" s="50">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
     </row>
-    <row r="8" ht="42.75" spans="2:11">
-      <c r="B8" s="51" t="s">
+    <row r="8" spans="1:11" ht="45">
+      <c r="B8" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="52" t="s">
+      <c r="C8" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="51">
+      <c r="D8" s="46">
         <v>5</v>
       </c>
-      <c r="E8" s="51">
+      <c r="E8" s="46">
         <v>5</v>
       </c>
-      <c r="F8" s="51">
+      <c r="F8" s="46">
         <v>5</v>
       </c>
-      <c r="G8" s="51">
+      <c r="G8" s="46">
         <v>1</v>
       </c>
-      <c r="H8" s="51">
+      <c r="H8" s="46">
         <v>4</v>
       </c>
-      <c r="I8" s="55">
+      <c r="I8" s="50">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="J8" s="55">
+      <c r="J8" s="50">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="K8" s="55">
+      <c r="K8" s="50">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
     </row>
-    <row r="9" ht="28.5" spans="2:11">
-      <c r="B9" s="51" t="s">
+    <row r="9" spans="1:11" ht="30">
+      <c r="B9" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="52" t="s">
+      <c r="C9" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="51">
+      <c r="D9" s="46">
         <v>2</v>
       </c>
-      <c r="E9" s="51">
+      <c r="E9" s="46">
         <v>2</v>
       </c>
-      <c r="F9" s="51">
+      <c r="F9" s="46">
         <v>2</v>
       </c>
-      <c r="G9" s="51">
+      <c r="G9" s="46">
         <v>7</v>
       </c>
-      <c r="H9" s="51">
+      <c r="H9" s="46">
         <v>1</v>
       </c>
-      <c r="I9" s="55">
+      <c r="I9" s="50">
         <f t="shared" si="0"/>
         <v>2.8</v>
       </c>
-      <c r="J9" s="55">
+      <c r="J9" s="50">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="K9" s="55">
+      <c r="K9" s="50">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
-    <row r="10" ht="42.75" spans="2:11">
-      <c r="B10" s="51" t="s">
+    <row r="10" spans="1:11" ht="45">
+      <c r="B10" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="52" t="s">
+      <c r="C10" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="51">
+      <c r="D10" s="46">
         <v>3</v>
       </c>
-      <c r="E10" s="51">
+      <c r="E10" s="46">
         <v>3</v>
       </c>
-      <c r="F10" s="51">
+      <c r="F10" s="46">
         <v>3</v>
       </c>
-      <c r="G10" s="51">
+      <c r="G10" s="46">
         <v>8</v>
       </c>
-      <c r="H10" s="51">
+      <c r="H10" s="46">
         <v>5</v>
       </c>
-      <c r="I10" s="55">
+      <c r="I10" s="50">
         <f t="shared" si="0"/>
-        <v>4.4</v>
-      </c>
-      <c r="J10" s="55">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="J10" s="50">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="K10" s="55">
+      <c r="K10" s="50">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
     </row>
-    <row r="11" ht="42.75" spans="2:11">
-      <c r="B11" s="51" t="s">
+    <row r="11" spans="1:11" ht="45">
+      <c r="B11" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="52" t="s">
+      <c r="C11" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="51">
+      <c r="D11" s="46">
         <v>1</v>
       </c>
-      <c r="E11" s="51">
+      <c r="E11" s="46">
         <v>1</v>
       </c>
-      <c r="F11" s="51">
+      <c r="F11" s="46">
         <v>1</v>
       </c>
-      <c r="G11" s="51">
+      <c r="G11" s="46">
         <v>9</v>
       </c>
-      <c r="H11" s="51">
+      <c r="H11" s="46">
         <v>2</v>
       </c>
-      <c r="I11" s="55">
+      <c r="I11" s="50">
         <f t="shared" si="0"/>
         <v>2.8</v>
       </c>
-      <c r="J11" s="55">
+      <c r="J11" s="50">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="K11" s="55">
+      <c r="K11" s="50">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="53" t="s">
+    <row r="13" spans="1:11" ht="15.75">
+      <c r="A13" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="53" t="s">
+      <c r="B13" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="53" t="s">
+      <c r="C13" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="50" t="s">
+      <c r="D13" s="45" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="50" t="s">
+    <row r="14" spans="1:11">
+      <c r="A14" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="54" t="s">
+      <c r="B14" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="54">
+      <c r="C14" s="49">
         <v>2.8</v>
       </c>
-      <c r="D14" s="51">
+      <c r="D14" s="46">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="50" t="s">
+    <row r="15" spans="1:11">
+      <c r="A15" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="54" t="s">
+      <c r="B15" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="54">
+      <c r="C15" s="49">
         <v>2.8</v>
       </c>
-      <c r="D15" s="51">
+      <c r="D15" s="46">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="50" t="s">
+    <row r="16" spans="1:11">
+      <c r="A16" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="51" t="s">
+      <c r="B16" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="51">
+      <c r="C16" s="46">
         <v>3.4</v>
       </c>
-      <c r="D16" s="51">
+      <c r="D16" s="46">
         <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="50" t="s">
+      <c r="A17" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="51" t="s">
+      <c r="B17" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="51">
+      <c r="C17" s="46">
         <v>4</v>
       </c>
-      <c r="D17" s="51">
+      <c r="D17" s="46">
         <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="50" t="s">
+      <c r="A18" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="51" t="s">
+      <c r="B18" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="51">
-        <v>4.4</v>
-      </c>
-      <c r="D18" s="51">
+      <c r="C18" s="46">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="D18" s="46">
         <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="50" t="s">
+      <c r="A19" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="51" t="s">
+      <c r="B19" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="51">
+      <c r="C19" s="46">
         <v>5.8</v>
       </c>
-      <c r="D19" s="51">
+      <c r="D19" s="46">
         <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="50" t="s">
+      <c r="A20" s="45" t="s">
         <v>35</v>
       </c>
-      <c r="B20" s="51" t="s">
+      <c r="B20" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="51">
+      <c r="C20" s="46">
         <v>6.6</v>
       </c>
-      <c r="D20" s="51">
+      <c r="D20" s="46">
         <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="50" t="s">
+      <c r="A21" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="B21" s="51" t="s">
+      <c r="B21" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="C21" s="51">
+      <c r="C21" s="46">
         <v>7.6</v>
       </c>
-      <c r="D21" s="51">
+      <c r="D21" s="46">
         <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="50" t="s">
+      <c r="A22" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="B22" s="51" t="s">
+      <c r="B22" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="51">
+      <c r="C22" s="46">
         <v>7.6</v>
       </c>
-      <c r="D22" s="51">
+      <c r="D22" s="46">
         <v>8</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="B14:C22">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B14:C22">
     <sortCondition ref="C14"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="7" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="13.375" customWidth="true"/>
-    <col min="3" max="3" width="11" customWidth="true"/>
-    <col min="4" max="4" width="10.625" customWidth="true"/>
-    <col min="5" max="5" width="12.25" customWidth="true"/>
-    <col min="6" max="6" width="9.375" customWidth="true"/>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:7">
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="50" t="s">
+      <c r="C2" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="50" t="s">
+      <c r="D2" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="50" t="s">
+      <c r="E2" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="50" t="s">
+      <c r="F2" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="50" t="s">
+      <c r="G2" s="45" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="2:7">
-      <c r="B3" s="51" t="s">
+      <c r="B3" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="51">
+      <c r="C3" s="46">
         <v>4</v>
       </c>
-      <c r="D3" s="51">
+      <c r="D3" s="46">
         <v>6</v>
       </c>
-      <c r="E3" s="51">
+      <c r="E3" s="46">
         <v>6</v>
       </c>
-      <c r="F3" s="51">
+      <c r="F3" s="46">
         <v>6</v>
       </c>
-      <c r="G3" s="51">
+      <c r="G3" s="46">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="2:7">
-      <c r="B4" s="51" t="s">
+      <c r="B4" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="51">
+      <c r="C4" s="46">
         <v>1</v>
       </c>
-      <c r="D4" s="51">
+      <c r="D4" s="46">
         <v>1</v>
       </c>
-      <c r="E4" s="51">
+      <c r="E4" s="46">
         <v>1</v>
       </c>
-      <c r="F4" s="51">
+      <c r="F4" s="46">
         <v>2</v>
       </c>
-      <c r="G4" s="51">
+      <c r="G4" s="46">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="2:7">
-      <c r="B5" s="51" t="s">
+      <c r="B5" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="51">
+      <c r="C5" s="46">
         <v>5</v>
       </c>
-      <c r="D5" s="51">
+      <c r="D5" s="46">
         <v>5</v>
       </c>
-      <c r="E5" s="51">
+      <c r="E5" s="46">
         <v>5</v>
       </c>
-      <c r="F5" s="51">
+      <c r="F5" s="46">
         <v>5</v>
       </c>
-      <c r="G5" s="51">
+      <c r="G5" s="46">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="2:7">
-      <c r="B6" s="51" t="s">
+      <c r="B6" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="51">
+      <c r="C6" s="46">
         <v>3</v>
       </c>
-      <c r="D6" s="51">
+      <c r="D6" s="46">
         <v>3</v>
       </c>
-      <c r="E6" s="51">
+      <c r="E6" s="46">
         <v>3</v>
       </c>
-      <c r="F6" s="51">
+      <c r="F6" s="46">
         <v>3</v>
       </c>
-      <c r="G6" s="51">
+      <c r="G6" s="46">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="2:7">
-      <c r="B7" s="51" t="s">
+      <c r="B7" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="51">
+      <c r="C7" s="46">
         <v>6</v>
       </c>
-      <c r="D7" s="51">
+      <c r="D7" s="46">
         <v>4</v>
       </c>
-      <c r="E7" s="51">
+      <c r="E7" s="46">
         <v>4</v>
       </c>
-      <c r="F7" s="51">
+      <c r="F7" s="46">
         <v>4</v>
       </c>
-      <c r="G7" s="51">
+      <c r="G7" s="46">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="2:7">
-      <c r="B8" s="51" t="s">
+      <c r="B8" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="51">
+      <c r="C8" s="46">
         <v>2</v>
       </c>
-      <c r="D8" s="51">
+      <c r="D8" s="46">
         <v>2</v>
       </c>
-      <c r="E8" s="51">
+      <c r="E8" s="46">
         <v>2</v>
       </c>
-      <c r="F8" s="51">
+      <c r="F8" s="46">
         <v>1</v>
       </c>
-      <c r="G8" s="51">
+      <c r="G8" s="46">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AC34"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B14" sqref="B14:Z23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.81666666666667" customWidth="true"/>
-    <col min="2" max="2" width="9.85" customWidth="true"/>
-    <col min="3" max="3" width="8.225" customWidth="true"/>
-    <col min="4" max="4" width="1.15" customWidth="true"/>
-    <col min="5" max="5" width="7.5" customWidth="true"/>
-    <col min="6" max="6" width="2.125" customWidth="true"/>
-    <col min="7" max="7" width="1.175" customWidth="true"/>
-    <col min="8" max="8" width="8.675" customWidth="true"/>
-    <col min="9" max="9" width="1.34166666666667" customWidth="true"/>
-    <col min="10" max="10" width="8.675" customWidth="true"/>
-    <col min="11" max="11" width="2.125" customWidth="true"/>
-    <col min="12" max="12" width="1.175" customWidth="true"/>
-    <col min="13" max="13" width="8.375" customWidth="true"/>
-    <col min="14" max="14" width="1.15" customWidth="true"/>
-    <col min="15" max="15" width="8.225" customWidth="true"/>
-    <col min="16" max="16" width="2.125" customWidth="true"/>
-    <col min="17" max="17" width="1.175" customWidth="true"/>
-    <col min="18" max="18" width="8.675" customWidth="true"/>
-    <col min="19" max="19" width="1.05" customWidth="true"/>
-    <col min="20" max="20" width="8.36666666666667" customWidth="true"/>
-    <col min="21" max="21" width="2.35" customWidth="true"/>
-    <col min="22" max="22" width="1.31666666666667" customWidth="true"/>
-    <col min="23" max="23" width="8.81666666666667" customWidth="true"/>
-    <col min="24" max="24" width="1.15" customWidth="true"/>
-    <col min="25" max="25" width="8.825" customWidth="true"/>
-    <col min="26" max="26" width="2.35" customWidth="true"/>
-    <col min="27" max="27" width="2.625" customWidth="true"/>
-    <col min="29" max="29" width="4.10833333333333" customWidth="true"/>
+    <col min="1" max="1" width="3.85546875" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" customWidth="1"/>
+    <col min="3" max="3" width="8.28515625" customWidth="1"/>
+    <col min="4" max="4" width="1.140625" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" customWidth="1"/>
+    <col min="6" max="6" width="2.140625" customWidth="1"/>
+    <col min="7" max="7" width="1.140625" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" customWidth="1"/>
+    <col min="9" max="9" width="1.28515625" customWidth="1"/>
+    <col min="10" max="10" width="8.7109375" customWidth="1"/>
+    <col min="11" max="11" width="2.140625" customWidth="1"/>
+    <col min="12" max="12" width="1.140625" customWidth="1"/>
+    <col min="13" max="13" width="8.42578125" customWidth="1"/>
+    <col min="14" max="14" width="1.140625" customWidth="1"/>
+    <col min="15" max="15" width="8.28515625" customWidth="1"/>
+    <col min="16" max="16" width="2.140625" customWidth="1"/>
+    <col min="17" max="17" width="1.140625" customWidth="1"/>
+    <col min="18" max="18" width="8.7109375" customWidth="1"/>
+    <col min="19" max="19" width="1" customWidth="1"/>
+    <col min="20" max="20" width="8.42578125" customWidth="1"/>
+    <col min="21" max="21" width="2.28515625" customWidth="1"/>
+    <col min="22" max="22" width="1.28515625" customWidth="1"/>
+    <col min="23" max="23" width="8.85546875" customWidth="1"/>
+    <col min="24" max="24" width="1.140625" customWidth="1"/>
+    <col min="25" max="25" width="8.85546875" customWidth="1"/>
+    <col min="26" max="26" width="2.28515625" customWidth="1"/>
+    <col min="27" max="27" width="2.5703125" customWidth="1"/>
+    <col min="29" max="29" width="4.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="12" customHeight="true" spans="1:29">
+    <row r="1" spans="1:29" ht="12" customHeight="1">
       <c r="A1" s="7"/>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -3954,175 +3374,175 @@
       <c r="Y1" s="7"/>
       <c r="Z1" s="7"/>
       <c r="AA1" s="7"/>
-      <c r="AC1" s="22"/>
-    </row>
-    <row r="2" ht="27" customHeight="true" spans="1:29">
+      <c r="AC1" s="18"/>
+    </row>
+    <row r="2" spans="1:29" ht="27" customHeight="1">
       <c r="A2" s="7"/>
       <c r="B2" s="7"/>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="9" t="s">
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="22"/>
-      <c r="M2" s="9" t="s">
+      <c r="I2" s="52"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
-      <c r="P2" s="21"/>
-      <c r="Q2" s="22"/>
-      <c r="R2" s="9" t="s">
+      <c r="N2" s="52"/>
+      <c r="O2" s="52"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="18"/>
+      <c r="R2" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="S2" s="10"/>
-      <c r="T2" s="10"/>
-      <c r="U2" s="21"/>
-      <c r="V2" s="22"/>
-      <c r="W2" s="9" t="s">
+      <c r="S2" s="52"/>
+      <c r="T2" s="52"/>
+      <c r="U2" s="53"/>
+      <c r="V2" s="18"/>
+      <c r="W2" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="X2" s="10"/>
-      <c r="Y2" s="10"/>
-      <c r="Z2" s="21"/>
-      <c r="AA2" s="22"/>
-      <c r="AB2" s="21" t="s">
+      <c r="X2" s="52"/>
+      <c r="Y2" s="52"/>
+      <c r="Z2" s="53"/>
+      <c r="AA2" s="18"/>
+      <c r="AB2" s="17" t="s">
         <v>43</v>
       </c>
       <c r="AC2" s="8"/>
     </row>
-    <row r="3" ht="24" customHeight="true" spans="1:29">
+    <row r="3" spans="1:29" ht="24" customHeight="1">
       <c r="A3" s="7"/>
       <c r="B3" s="7"/>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="12"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="24" t="s">
+      <c r="D3" s="55"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="19" t="s">
         <v>28</v>
       </c>
       <c r="G3" s="8"/>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="I3" s="12"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="24" t="s">
+      <c r="I3" s="55"/>
+      <c r="J3" s="56"/>
+      <c r="K3" s="19" t="s">
         <v>28</v>
       </c>
       <c r="L3" s="8"/>
-      <c r="M3" s="11" t="s">
+      <c r="M3" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="N3" s="12"/>
-      <c r="O3" s="23"/>
-      <c r="P3" s="24" t="s">
+      <c r="N3" s="55"/>
+      <c r="O3" s="56"/>
+      <c r="P3" s="19" t="s">
         <v>28</v>
       </c>
       <c r="Q3" s="8"/>
-      <c r="R3" s="11" t="s">
+      <c r="R3" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="S3" s="12"/>
-      <c r="T3" s="23"/>
-      <c r="U3" s="24" t="s">
+      <c r="S3" s="55"/>
+      <c r="T3" s="56"/>
+      <c r="U3" s="19" t="s">
         <v>28</v>
       </c>
       <c r="V3" s="8"/>
-      <c r="W3" s="11" t="s">
+      <c r="W3" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="X3" s="12"/>
-      <c r="Y3" s="23"/>
-      <c r="Z3" s="24" t="s">
+      <c r="X3" s="55"/>
+      <c r="Y3" s="56"/>
+      <c r="Z3" s="19" t="s">
         <v>28</v>
       </c>
       <c r="AA3" s="8"/>
-      <c r="AB3" s="24" t="s">
+      <c r="AB3" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="AC3" s="22"/>
+      <c r="AC3" s="18"/>
     </row>
     <row r="4" spans="1:29">
       <c r="A4" s="7"/>
       <c r="B4" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="13">
-        <v>0.132</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="E4" s="25">
-        <v>0.0965063776002464</v>
-      </c>
-      <c r="F4" s="22">
+      <c r="C4" s="9">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="20">
+        <v>9.6506377600246399E-2</v>
+      </c>
+      <c r="F4" s="18">
         <v>4</v>
       </c>
-      <c r="G4" s="22"/>
-      <c r="H4" s="13">
+      <c r="G4" s="18"/>
+      <c r="H4" s="9">
         <v>19.273</v>
       </c>
-      <c r="I4" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="J4" s="36">
-        <v>4.36737875829437</v>
-      </c>
-      <c r="K4" s="22">
+      <c r="I4" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="J4" s="31">
+        <v>4.3673787582943699</v>
+      </c>
+      <c r="K4" s="18">
         <v>4</v>
       </c>
-      <c r="L4" s="22"/>
-      <c r="M4" s="41">
-        <v>3.19134547909331e-5</v>
-      </c>
-      <c r="N4" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="O4" s="40">
-        <v>4.53693404059032e-5</v>
-      </c>
-      <c r="P4" s="42">
+      <c r="L4" s="18"/>
+      <c r="M4" s="36">
+        <v>3.1913454790933101E-5</v>
+      </c>
+      <c r="N4" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="O4" s="35">
+        <v>4.5369340405903198E-5</v>
+      </c>
+      <c r="P4" s="37">
         <v>1</v>
       </c>
-      <c r="Q4" s="22"/>
-      <c r="R4" s="13">
-        <v>536.477</v>
-      </c>
-      <c r="S4" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="T4" s="36">
+      <c r="Q4" s="18"/>
+      <c r="R4" s="9">
+        <v>536.47699999999998</v>
+      </c>
+      <c r="S4" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="T4" s="31">
         <v>196.069181001229</v>
       </c>
-      <c r="U4" s="22">
+      <c r="U4" s="18">
         <v>4</v>
       </c>
-      <c r="V4" s="22"/>
-      <c r="W4" s="41">
-        <v>0.276</v>
-      </c>
-      <c r="X4" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="Y4" s="40">
-        <v>0.798042531991864</v>
-      </c>
-      <c r="Z4" s="42">
+      <c r="V4" s="18"/>
+      <c r="W4" s="36">
+        <v>0.27600000000000002</v>
+      </c>
+      <c r="X4" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y4" s="35">
+        <v>0.79804253199186403</v>
+      </c>
+      <c r="Z4" s="37">
         <v>2</v>
       </c>
-      <c r="AA4" s="22"/>
-      <c r="AB4" s="22">
+      <c r="AA4" s="18"/>
+      <c r="AB4" s="18">
         <f t="shared" ref="AB4:AB9" si="0">AVERAGE(F4,K4,P4,U4,Z4)</f>
         <v>3</v>
       </c>
@@ -4133,72 +3553,72 @@
       <c r="B5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="15">
-        <v>0.009</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="E5" s="26">
-        <v>0.0122558806800694</v>
-      </c>
-      <c r="F5" s="27">
+      <c r="C5" s="11">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="21">
+        <v>1.22558806800694E-2</v>
+      </c>
+      <c r="F5" s="22">
         <v>2</v>
       </c>
       <c r="G5" s="8"/>
-      <c r="H5" s="15">
-        <v>8.206</v>
-      </c>
-      <c r="I5" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="J5" s="37">
-        <v>3.16209259736571</v>
-      </c>
-      <c r="K5" s="27">
+      <c r="H5" s="11">
+        <v>8.2059999999999995</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="J5" s="32">
+        <v>3.1620925973657101</v>
+      </c>
+      <c r="K5" s="22">
         <v>1</v>
       </c>
       <c r="L5" s="8"/>
-      <c r="M5" s="17">
-        <v>4.64721586113555e-5</v>
-      </c>
-      <c r="N5" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="O5" s="43">
-        <v>3.52283254856238e-5</v>
+      <c r="M5" s="13">
+        <v>4.64721586113555E-5</v>
+      </c>
+      <c r="N5" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="O5" s="38">
+        <v>3.52283254856238E-5</v>
       </c>
       <c r="P5" s="8">
         <v>4</v>
       </c>
       <c r="Q5" s="8"/>
-      <c r="R5" s="15">
-        <v>168.007</v>
-      </c>
-      <c r="S5" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="T5" s="46">
+      <c r="R5" s="11">
+        <v>168.00700000000001</v>
+      </c>
+      <c r="S5" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="T5" s="41">
         <v>108.236426929137</v>
       </c>
-      <c r="U5" s="27">
+      <c r="U5" s="22">
         <v>2</v>
       </c>
       <c r="V5" s="8"/>
-      <c r="W5" s="15">
+      <c r="W5" s="11">
         <v>0.2</v>
       </c>
-      <c r="X5" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="Y5" s="40">
-        <v>0.531586549460241</v>
-      </c>
-      <c r="Z5" s="27">
+      <c r="X5" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y5" s="35">
+        <v>0.53158654946024098</v>
+      </c>
+      <c r="Z5" s="22">
         <v>1</v>
       </c>
       <c r="AA5" s="8"/>
-      <c r="AB5" s="42">
+      <c r="AB5" s="37">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
@@ -4209,72 +3629,72 @@
       <c r="B6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="17">
+      <c r="C6" s="13">
         <v>0.996</v>
       </c>
-      <c r="D6" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="E6" s="25">
-        <v>0.579582288921128</v>
+      <c r="D6" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="20">
+        <v>0.57958228892112795</v>
       </c>
       <c r="F6" s="8">
         <v>5</v>
       </c>
       <c r="G6" s="8"/>
-      <c r="H6" s="17">
-        <v>23.297</v>
-      </c>
-      <c r="I6" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="J6" s="36">
-        <v>8.49956838329015</v>
+      <c r="H6" s="13">
+        <v>23.297000000000001</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="J6" s="31">
+        <v>8.4995683832901499</v>
       </c>
       <c r="K6" s="8">
         <v>5</v>
       </c>
       <c r="L6" s="8"/>
-      <c r="M6" s="17">
-        <v>0.000103390053282981</v>
-      </c>
-      <c r="N6" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="O6" s="43">
-        <v>0.000149680503438306</v>
+      <c r="M6" s="13">
+        <v>1.03390053282981E-4</v>
+      </c>
+      <c r="N6" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="O6" s="38">
+        <v>1.4968050343830601E-4</v>
       </c>
       <c r="P6" s="8">
         <v>5</v>
       </c>
       <c r="Q6" s="8"/>
-      <c r="R6" s="17">
-        <v>689.955</v>
-      </c>
-      <c r="S6" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="T6" s="36">
+      <c r="R6" s="13">
+        <v>689.95500000000004</v>
+      </c>
+      <c r="S6" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="T6" s="31">
         <v>246.763475736191</v>
       </c>
       <c r="U6" s="8">
         <v>5</v>
       </c>
       <c r="V6" s="8"/>
-      <c r="W6" s="17">
-        <v>5.752</v>
-      </c>
-      <c r="X6" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="Y6" s="43">
-        <v>3.69881847868128</v>
+      <c r="W6" s="13">
+        <v>5.7519999999999998</v>
+      </c>
+      <c r="X6" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y6" s="38">
+        <v>3.6988184786812801</v>
       </c>
       <c r="Z6" s="8">
         <v>6</v>
       </c>
       <c r="AA6" s="8"/>
-      <c r="AB6" s="22">
+      <c r="AB6" s="18">
         <f t="shared" si="0"/>
         <v>5.2</v>
       </c>
@@ -4285,72 +3705,72 @@
       <c r="B7" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="17">
-        <v>0.088</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="E7" s="25">
-        <v>0.0657868338421766</v>
+      <c r="C7" s="13">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="20">
+        <v>6.5786833842176595E-2</v>
       </c>
       <c r="F7" s="8">
         <v>3</v>
       </c>
       <c r="G7" s="8"/>
-      <c r="H7" s="17">
+      <c r="H7" s="13">
         <v>15.849</v>
       </c>
-      <c r="I7" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="J7" s="36">
-        <v>4.63424091289783</v>
+      <c r="I7" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="J7" s="31">
+        <v>4.6342409128978304</v>
       </c>
       <c r="K7" s="8">
         <v>3</v>
       </c>
       <c r="L7" s="8"/>
-      <c r="M7" s="15">
-        <v>4.16744416210794e-5</v>
-      </c>
-      <c r="N7" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="O7" s="40">
-        <v>4.13442717575075e-5</v>
-      </c>
-      <c r="P7" s="27">
+      <c r="M7" s="11">
+        <v>4.1674441621079401E-5</v>
+      </c>
+      <c r="N7" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="O7" s="35">
+        <v>4.1344271757507498E-5</v>
+      </c>
+      <c r="P7" s="22">
         <v>2</v>
       </c>
       <c r="Q7" s="8"/>
-      <c r="R7" s="17">
+      <c r="R7" s="13">
         <v>525.29</v>
       </c>
-      <c r="S7" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="T7" s="47">
-        <v>179.800681426741</v>
+      <c r="S7" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="T7" s="42">
+        <v>179.80068142674099</v>
       </c>
       <c r="U7" s="8">
         <v>3</v>
       </c>
       <c r="V7" s="8"/>
-      <c r="W7" s="17">
-        <v>0.645</v>
-      </c>
-      <c r="X7" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="Y7" s="43">
-        <v>0.763103960603693</v>
+      <c r="W7" s="13">
+        <v>0.64500000000000002</v>
+      </c>
+      <c r="X7" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y7" s="38">
+        <v>0.76310396060369301</v>
       </c>
       <c r="Z7" s="8">
         <v>3</v>
       </c>
       <c r="AA7" s="8"/>
-      <c r="AB7" s="22">
+      <c r="AB7" s="18">
         <f t="shared" si="0"/>
         <v>2.8</v>
       </c>
@@ -4361,72 +3781,72 @@
       <c r="B8" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="17">
-        <v>1.787</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="E8" s="25">
-        <v>1.84905922972114</v>
+      <c r="C8" s="13">
+        <v>1.7869999999999999</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="20">
+        <v>1.8490592297211399</v>
       </c>
       <c r="F8" s="8">
         <v>6</v>
       </c>
       <c r="G8" s="8"/>
-      <c r="H8" s="17">
+      <c r="H8" s="13">
         <v>26.581</v>
       </c>
-      <c r="I8" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="J8" s="36">
-        <v>9.62226037415531</v>
+      <c r="I8" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="J8" s="31">
+        <v>9.6222603741553101</v>
       </c>
       <c r="K8" s="8">
         <v>6</v>
       </c>
       <c r="L8" s="8"/>
-      <c r="M8" s="17">
-        <v>0.000165280623744032</v>
-      </c>
-      <c r="N8" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="O8" s="43">
-        <v>0.000243528763630911</v>
+      <c r="M8" s="13">
+        <v>1.65280623744032E-4</v>
+      </c>
+      <c r="N8" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="O8" s="38">
+        <v>2.4352876363091099E-4</v>
       </c>
       <c r="P8" s="8">
         <v>6</v>
       </c>
       <c r="Q8" s="8"/>
-      <c r="R8" s="17">
+      <c r="R8" s="13">
         <v>793.303</v>
       </c>
-      <c r="S8" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="T8" s="36">
+      <c r="S8" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="T8" s="31">
         <v>150.270527086389</v>
       </c>
       <c r="U8" s="8">
         <v>6</v>
       </c>
       <c r="V8" s="8"/>
-      <c r="W8" s="17">
-        <v>2.704</v>
-      </c>
-      <c r="X8" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="Y8" s="43">
-        <v>3.5720431699787</v>
+      <c r="W8" s="13">
+        <v>2.7040000000000002</v>
+      </c>
+      <c r="X8" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y8" s="38">
+        <v>3.5720431699786999</v>
       </c>
       <c r="Z8" s="8">
         <v>5</v>
       </c>
       <c r="AA8" s="8"/>
-      <c r="AB8" s="22">
+      <c r="AB8" s="18">
         <f t="shared" si="0"/>
         <v>5.8</v>
       </c>
@@ -4437,74 +3857,74 @@
       <c r="B9" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="15">
-        <v>0.007</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="E9" s="26">
-        <v>0.00678518699644487</v>
-      </c>
-      <c r="F9" s="27">
+      <c r="C9" s="11">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9" s="21">
+        <v>6.7851869964448697E-3</v>
+      </c>
+      <c r="F9" s="22">
         <v>1</v>
       </c>
       <c r="G9" s="8"/>
-      <c r="H9" s="15">
-        <v>8.249</v>
-      </c>
-      <c r="I9" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="J9" s="37">
-        <v>2.66170675596635</v>
-      </c>
-      <c r="K9" s="27">
+      <c r="H9" s="11">
+        <v>8.2490000000000006</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="J9" s="32">
+        <v>2.6617067559663501</v>
+      </c>
+      <c r="K9" s="22">
         <v>2</v>
       </c>
       <c r="L9" s="8"/>
-      <c r="M9" s="17">
-        <v>4.35533283922469e-5</v>
-      </c>
-      <c r="N9" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="O9" s="43">
-        <v>4.94646892158851e-5</v>
+      <c r="M9" s="13">
+        <v>4.3553328392246902E-5</v>
+      </c>
+      <c r="N9" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="O9" s="38">
+        <v>4.9464689215885101E-5</v>
       </c>
       <c r="P9" s="8">
         <v>3</v>
       </c>
       <c r="Q9" s="8"/>
-      <c r="R9" s="15">
-        <v>151.254</v>
-      </c>
-      <c r="S9" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="T9" s="46">
+      <c r="R9" s="11">
+        <v>151.25399999999999</v>
+      </c>
+      <c r="S9" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="T9" s="41">
         <v>103.795401126775</v>
       </c>
-      <c r="U9" s="27">
+      <c r="U9" s="22">
         <v>1</v>
       </c>
       <c r="V9" s="8"/>
-      <c r="W9" s="17">
-        <v>0.963</v>
-      </c>
-      <c r="X9" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="Y9" s="43">
-        <v>0.742071728255402</v>
+      <c r="W9" s="13">
+        <v>0.96299999999999997</v>
+      </c>
+      <c r="X9" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y9" s="38">
+        <v>0.74207172825540202</v>
       </c>
       <c r="Z9" s="8">
         <v>4</v>
       </c>
       <c r="AA9" s="8"/>
-      <c r="AB9" s="42">
+      <c r="AB9" s="37">
         <f t="shared" si="0"/>
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="AC9" s="8"/>
     </row>
@@ -4583,9 +4003,9 @@
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
       <c r="L12" s="8"/>
-      <c r="M12" s="44"/>
+      <c r="M12" s="39"/>
       <c r="N12" s="8"/>
-      <c r="O12" s="45"/>
+      <c r="O12" s="40"/>
       <c r="P12" s="7"/>
       <c r="Q12" s="7"/>
       <c r="R12" s="7"/>
@@ -4601,510 +4021,510 @@
       <c r="AB12" s="8"/>
       <c r="AC12" s="8"/>
     </row>
-    <row r="13" spans="8:12">
-      <c r="H13" s="28"/>
-      <c r="I13" s="28"/>
-      <c r="J13" s="28"/>
-      <c r="L13" s="38"/>
-    </row>
-    <row r="14" spans="1:27">
+    <row r="13" spans="1:29">
+      <c r="H13" s="23"/>
+      <c r="I13" s="23"/>
+      <c r="J13" s="23"/>
+      <c r="L13" s="33"/>
+    </row>
+    <row r="14" spans="1:29">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="10"/>
-      <c r="N14" s="10"/>
-      <c r="O14" s="10"/>
-      <c r="P14" s="10"/>
-      <c r="Q14" s="10"/>
-      <c r="R14" s="10"/>
-      <c r="S14" s="10"/>
-      <c r="T14" s="10"/>
-      <c r="U14" s="10"/>
-      <c r="V14" s="10"/>
-      <c r="W14" s="10"/>
-      <c r="X14" s="10"/>
-      <c r="Y14" s="10"/>
-      <c r="Z14" s="21"/>
+      <c r="D14" s="52"/>
+      <c r="E14" s="52"/>
+      <c r="F14" s="52"/>
+      <c r="G14" s="52"/>
+      <c r="H14" s="52"/>
+      <c r="I14" s="52"/>
+      <c r="J14" s="52"/>
+      <c r="K14" s="52"/>
+      <c r="L14" s="52"/>
+      <c r="M14" s="52"/>
+      <c r="N14" s="52"/>
+      <c r="O14" s="52"/>
+      <c r="P14" s="52"/>
+      <c r="Q14" s="52"/>
+      <c r="R14" s="52"/>
+      <c r="S14" s="52"/>
+      <c r="T14" s="52"/>
+      <c r="U14" s="52"/>
+      <c r="V14" s="52"/>
+      <c r="W14" s="52"/>
+      <c r="X14" s="52"/>
+      <c r="Y14" s="52"/>
+      <c r="Z14" s="53"/>
       <c r="AA14" s="7"/>
     </row>
-    <row r="15" spans="1:28">
+    <row r="15" spans="1:29">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="54" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="11" t="s">
+      <c r="D15" s="55"/>
+      <c r="E15" s="55"/>
+      <c r="F15" s="56"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
-      <c r="K15" s="23"/>
-      <c r="L15" s="22"/>
-      <c r="M15" s="11" t="s">
+      <c r="I15" s="55"/>
+      <c r="J15" s="55"/>
+      <c r="K15" s="56"/>
+      <c r="L15" s="18"/>
+      <c r="M15" s="54" t="s">
         <v>40</v>
       </c>
-      <c r="N15" s="12"/>
-      <c r="O15" s="12"/>
-      <c r="P15" s="23"/>
-      <c r="Q15" s="22"/>
-      <c r="R15" s="11" t="s">
+      <c r="N15" s="55"/>
+      <c r="O15" s="55"/>
+      <c r="P15" s="56"/>
+      <c r="Q15" s="18"/>
+      <c r="R15" s="54" t="s">
         <v>41</v>
       </c>
-      <c r="S15" s="12"/>
-      <c r="T15" s="12"/>
-      <c r="U15" s="23"/>
-      <c r="V15" s="22"/>
-      <c r="W15" s="11" t="s">
+      <c r="S15" s="55"/>
+      <c r="T15" s="55"/>
+      <c r="U15" s="56"/>
+      <c r="V15" s="18"/>
+      <c r="W15" s="54" t="s">
         <v>42</v>
       </c>
-      <c r="X15" s="12"/>
-      <c r="Y15" s="12"/>
-      <c r="Z15" s="23"/>
-      <c r="AA15" s="22"/>
-      <c r="AB15" s="22"/>
-    </row>
-    <row r="16" spans="1:28">
+      <c r="X15" s="55"/>
+      <c r="Y15" s="55"/>
+      <c r="Z15" s="56"/>
+      <c r="AA15" s="18"/>
+      <c r="AB15" s="18"/>
+    </row>
+    <row r="16" spans="1:29" ht="18">
       <c r="A16" s="7"/>
       <c r="B16" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C16" s="18">
+      <c r="C16" s="14">
         <v>0.114747845625917</v>
       </c>
-      <c r="D16" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="E16" s="29">
-        <v>0.0684432760067935</v>
-      </c>
-      <c r="F16" s="30" t="s">
+      <c r="D16" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" s="24">
+        <v>6.8443276006793494E-2</v>
+      </c>
+      <c r="F16" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="G16" s="31"/>
-      <c r="H16" s="18">
-        <v>19.6272217654338</v>
-      </c>
-      <c r="I16" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="J16" s="39">
-        <v>5.327205749671</v>
-      </c>
-      <c r="K16" s="30" t="s">
+      <c r="G16" s="26"/>
+      <c r="H16" s="14">
+        <v>19.627221765433799</v>
+      </c>
+      <c r="I16" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="J16" s="34">
+        <v>5.3272057496710001</v>
+      </c>
+      <c r="K16" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="L16" s="31"/>
-      <c r="M16" s="18">
-        <v>4.55652312635843e-5</v>
-      </c>
-      <c r="N16" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="O16" s="39">
-        <v>5.0571838413492e-5</v>
-      </c>
-      <c r="P16" s="30" t="s">
+      <c r="L16" s="26"/>
+      <c r="M16" s="14">
+        <v>4.55652312635843E-5</v>
+      </c>
+      <c r="N16" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="O16" s="34">
+        <v>5.0571838413492001E-5</v>
+      </c>
+      <c r="P16" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="Q16" s="31"/>
-      <c r="R16" s="18">
-        <v>524.062381716945</v>
-      </c>
-      <c r="S16" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="T16" s="48">
+      <c r="Q16" s="26"/>
+      <c r="R16" s="14">
+        <v>524.06238171694497</v>
+      </c>
+      <c r="S16" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="T16" s="43">
         <v>203.075140130466</v>
       </c>
-      <c r="U16" s="30" t="s">
+      <c r="U16" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="V16" s="31"/>
-      <c r="W16" s="18">
-        <v>0.58100670103607</v>
-      </c>
-      <c r="X16" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="Y16" s="39">
-        <v>0.822959171889959</v>
-      </c>
-      <c r="Z16" s="30" t="s">
+      <c r="V16" s="26"/>
+      <c r="W16" s="14">
+        <v>0.58100670103606999</v>
+      </c>
+      <c r="X16" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y16" s="34">
+        <v>0.82295917188995904</v>
+      </c>
+      <c r="Z16" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="AA16" s="22"/>
-      <c r="AB16" s="22"/>
-    </row>
-    <row r="17" spans="1:28">
+      <c r="AA16" s="18"/>
+      <c r="AB16" s="18"/>
+    </row>
+    <row r="17" spans="1:28" ht="18">
       <c r="A17" s="7"/>
       <c r="B17" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="20">
-        <v>0.0124808462079064</v>
-      </c>
-      <c r="D17" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="E17" s="29">
-        <v>0.0131805075558143</v>
-      </c>
-      <c r="F17" s="32" t="s">
+      <c r="C17" s="16">
+        <v>1.2480846207906401E-2</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="E17" s="24">
+        <v>1.31805075558143E-2</v>
+      </c>
+      <c r="F17" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="G17" s="33"/>
-      <c r="H17" s="20">
-        <v>8.96490632339721</v>
-      </c>
-      <c r="I17" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="J17" s="39">
+      <c r="G17" s="28"/>
+      <c r="H17" s="16">
+        <v>8.9649063233972104</v>
+      </c>
+      <c r="I17" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="J17" s="34">
         <v>2.75855365951938</v>
       </c>
-      <c r="K17" s="32" t="s">
+      <c r="K17" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="L17" s="33"/>
-      <c r="M17" s="20">
-        <v>4.18960602378896e-5</v>
-      </c>
-      <c r="N17" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="O17" s="39">
-        <v>3.92664893129244e-5</v>
-      </c>
-      <c r="P17" s="32" t="s">
+      <c r="L17" s="28"/>
+      <c r="M17" s="16">
+        <v>4.18960602378896E-5</v>
+      </c>
+      <c r="N17" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="O17" s="34">
+        <v>3.92664893129244E-5</v>
+      </c>
+      <c r="P17" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="Q17" s="33"/>
-      <c r="R17" s="20">
-        <v>194.075879224546</v>
-      </c>
-      <c r="S17" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="T17" s="49">
-        <v>125.897671391498</v>
-      </c>
-      <c r="U17" s="32" t="s">
+      <c r="Q17" s="28"/>
+      <c r="R17" s="16">
+        <v>194.07587922454599</v>
+      </c>
+      <c r="S17" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="T17" s="44">
+        <v>125.89767139149799</v>
+      </c>
+      <c r="U17" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="V17" s="33"/>
-      <c r="W17" s="15">
+      <c r="V17" s="28"/>
+      <c r="W17" s="11">
         <v>0.158863878668073</v>
       </c>
-      <c r="X17" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="Y17" s="40">
-        <v>0.468283259433261</v>
-      </c>
-      <c r="Z17" s="34" t="s">
+      <c r="X17" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y17" s="35">
+        <v>0.46828325943326099</v>
+      </c>
+      <c r="Z17" s="29" t="s">
         <v>47</v>
       </c>
       <c r="AA17" s="8"/>
       <c r="AB17" s="8"/>
     </row>
-    <row r="18" spans="1:28">
+    <row r="18" spans="1:28" ht="18">
       <c r="A18" s="7"/>
       <c r="B18" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="20">
+      <c r="C18" s="16">
         <v>1.05159177989402</v>
       </c>
-      <c r="D18" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="E18" s="29">
-        <v>0.611622928892933</v>
-      </c>
-      <c r="F18" s="32" t="s">
+      <c r="D18" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="E18" s="24">
+        <v>0.61162292889293302</v>
+      </c>
+      <c r="F18" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="G18" s="33"/>
-      <c r="H18" s="20">
-        <v>21.9147590599884</v>
-      </c>
-      <c r="I18" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="J18" s="39">
-        <v>7.5814931282509</v>
-      </c>
-      <c r="K18" s="32" t="s">
+      <c r="G18" s="28"/>
+      <c r="H18" s="16">
+        <v>21.914759059988398</v>
+      </c>
+      <c r="I18" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="J18" s="34">
+        <v>7.5814931282508997</v>
+      </c>
+      <c r="K18" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="L18" s="33"/>
-      <c r="M18" s="20">
-        <v>0.000108779608432157</v>
-      </c>
-      <c r="N18" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="O18" s="39">
-        <v>0.000109994849086413</v>
-      </c>
-      <c r="P18" s="32" t="s">
+      <c r="L18" s="28"/>
+      <c r="M18" s="16">
+        <v>1.08779608432157E-4</v>
+      </c>
+      <c r="N18" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="O18" s="34">
+        <v>1.09994849086413E-4</v>
+      </c>
+      <c r="P18" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="Q18" s="33"/>
-      <c r="R18" s="20">
-        <v>677.637046625668</v>
-      </c>
-      <c r="S18" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="T18" s="48">
-        <v>258.237746993981</v>
-      </c>
-      <c r="U18" s="32" t="s">
+      <c r="Q18" s="28"/>
+      <c r="R18" s="16">
+        <v>677.63704662566795</v>
+      </c>
+      <c r="S18" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="T18" s="43">
+        <v>258.23774699398098</v>
+      </c>
+      <c r="U18" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="V18" s="33"/>
-      <c r="W18" s="20">
+      <c r="V18" s="28"/>
+      <c r="W18" s="16">
         <v>5.84244063013593</v>
       </c>
-      <c r="X18" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="Y18" s="39">
-        <v>3.08203297399199</v>
-      </c>
-      <c r="Z18" s="32" t="s">
+      <c r="X18" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y18" s="34">
+        <v>3.0820329739919901</v>
+      </c>
+      <c r="Z18" s="27" t="s">
         <v>49</v>
       </c>
       <c r="AA18" s="8"/>
       <c r="AB18" s="8"/>
     </row>
-    <row r="19" spans="1:28">
+    <row r="19" spans="1:28" ht="18">
       <c r="A19" s="7"/>
       <c r="B19" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="20">
-        <v>0.0874221668089744</v>
-      </c>
-      <c r="D19" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="E19" s="29">
-        <v>0.0582475511981321</v>
-      </c>
-      <c r="F19" s="32" t="s">
+      <c r="C19" s="16">
+        <v>8.7422166808974397E-2</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" s="24">
+        <v>5.8247551198132103E-2</v>
+      </c>
+      <c r="F19" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="G19" s="33"/>
-      <c r="H19" s="20">
-        <v>16.589514851023</v>
-      </c>
-      <c r="I19" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="J19" s="39">
-        <v>4.77978244572968</v>
-      </c>
-      <c r="K19" s="32" t="s">
+      <c r="G19" s="28"/>
+      <c r="H19" s="16">
+        <v>16.589514851023001</v>
+      </c>
+      <c r="I19" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="J19" s="34">
+        <v>4.7797824457296798</v>
+      </c>
+      <c r="K19" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="L19" s="33"/>
-      <c r="M19" s="15">
-        <v>2.88602719669648e-5</v>
-      </c>
-      <c r="N19" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="O19" s="40">
-        <v>3.61923534155067e-5</v>
-      </c>
-      <c r="P19" s="34" t="s">
+      <c r="L19" s="28"/>
+      <c r="M19" s="11">
+        <v>2.8860271966964799E-5</v>
+      </c>
+      <c r="N19" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="O19" s="35">
+        <v>3.61923534155067E-5</v>
+      </c>
+      <c r="P19" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="Q19" s="33"/>
-      <c r="R19" s="20">
-        <v>494.569825205012</v>
-      </c>
-      <c r="S19" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="T19" s="49">
-        <v>152.911310080766</v>
-      </c>
-      <c r="U19" s="32" t="s">
+      <c r="Q19" s="28"/>
+      <c r="R19" s="16">
+        <v>494.56982520501202</v>
+      </c>
+      <c r="S19" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="T19" s="44">
+        <v>152.91131008076599</v>
+      </c>
+      <c r="U19" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="V19" s="33"/>
-      <c r="W19" s="20">
+      <c r="V19" s="28"/>
+      <c r="W19" s="16">
         <v>0.593830166653466</v>
       </c>
-      <c r="X19" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="Y19" s="39">
+      <c r="X19" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y19" s="34">
         <v>0.73938605960129</v>
       </c>
-      <c r="Z19" s="32" t="s">
+      <c r="Z19" s="27" t="s">
         <v>47</v>
       </c>
       <c r="AA19" s="8"/>
       <c r="AB19" s="8"/>
     </row>
-    <row r="20" spans="1:28">
+    <row r="20" spans="1:28" ht="18">
       <c r="A20" s="7"/>
       <c r="B20" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="20">
-        <v>2.27881585519321</v>
-      </c>
-      <c r="D20" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="E20" s="29">
-        <v>2.26530329503765</v>
-      </c>
-      <c r="F20" s="32" t="s">
+      <c r="C20" s="16">
+        <v>2.2788158551932098</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="E20" s="24">
+        <v>2.2653032950376502</v>
+      </c>
+      <c r="F20" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="G20" s="33"/>
-      <c r="H20" s="20">
+      <c r="G20" s="28"/>
+      <c r="H20" s="16">
         <v>28.9257152387503</v>
       </c>
-      <c r="I20" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="J20" s="39">
-        <v>10.7084034758881</v>
-      </c>
-      <c r="K20" s="32" t="s">
+      <c r="I20" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="J20" s="34">
+        <v>10.708403475888099</v>
+      </c>
+      <c r="K20" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="L20" s="33"/>
-      <c r="M20" s="20">
-        <v>0.000161182677815521</v>
-      </c>
-      <c r="N20" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="O20" s="39">
-        <v>0.000201454522136078</v>
-      </c>
-      <c r="P20" s="32" t="s">
+      <c r="L20" s="28"/>
+      <c r="M20" s="16">
+        <v>1.61182677815521E-4</v>
+      </c>
+      <c r="N20" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="O20" s="34">
+        <v>2.01454522136078E-4</v>
+      </c>
+      <c r="P20" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="Q20" s="33"/>
-      <c r="R20" s="20">
-        <v>780.263415300589</v>
-      </c>
-      <c r="S20" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="T20" s="48">
-        <v>221.178220897061</v>
-      </c>
-      <c r="U20" s="32" t="s">
+      <c r="Q20" s="28"/>
+      <c r="R20" s="16">
+        <v>780.26341530058903</v>
+      </c>
+      <c r="S20" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="T20" s="43">
+        <v>221.17822089706101</v>
+      </c>
+      <c r="U20" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="V20" s="33"/>
-      <c r="W20" s="20">
-        <v>2.72833698273227</v>
-      </c>
-      <c r="X20" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="Y20" s="39">
-        <v>3.51381108641982</v>
-      </c>
-      <c r="Z20" s="32" t="s">
+      <c r="V20" s="28"/>
+      <c r="W20" s="16">
+        <v>2.7283369827322699</v>
+      </c>
+      <c r="X20" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y20" s="34">
+        <v>3.5138110864198202</v>
+      </c>
+      <c r="Z20" s="27" t="s">
         <v>52</v>
       </c>
       <c r="AA20" s="8"/>
       <c r="AB20" s="8"/>
     </row>
-    <row r="21" spans="1:28">
+    <row r="21" spans="1:28" ht="18">
       <c r="A21" s="7"/>
       <c r="B21" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="15">
-        <v>0.00722520327319471</v>
-      </c>
-      <c r="D21" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="E21" s="26">
-        <v>0.00848600342988601</v>
-      </c>
-      <c r="F21" s="34" t="s">
+      <c r="C21" s="11">
+        <v>7.2252032731947103E-3</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21" s="21">
+        <v>8.4860034298860094E-3</v>
+      </c>
+      <c r="F21" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="G21" s="33"/>
-      <c r="H21" s="15">
-        <v>7.45875253602551</v>
-      </c>
-      <c r="I21" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="J21" s="40">
-        <v>2.70397065899332</v>
-      </c>
-      <c r="K21" s="34" t="s">
+      <c r="G21" s="28"/>
+      <c r="H21" s="11">
+        <v>7.4587525360255098</v>
+      </c>
+      <c r="I21" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="J21" s="35">
+        <v>2.7039706589933199</v>
+      </c>
+      <c r="K21" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="L21" s="33"/>
-      <c r="M21" s="20">
-        <v>6.00430497488383e-5</v>
-      </c>
-      <c r="N21" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="O21" s="39">
-        <v>5.96314998905934e-5</v>
-      </c>
-      <c r="P21" s="32" t="s">
+      <c r="L21" s="28"/>
+      <c r="M21" s="16">
+        <v>6.0043049748838303E-5</v>
+      </c>
+      <c r="N21" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="O21" s="34">
+        <v>5.9631499890593403E-5</v>
+      </c>
+      <c r="P21" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="Q21" s="33"/>
-      <c r="R21" s="15">
-        <v>172.127171551962</v>
-      </c>
-      <c r="S21" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="T21" s="46">
+      <c r="Q21" s="28"/>
+      <c r="R21" s="11">
+        <v>172.12717155196199</v>
+      </c>
+      <c r="S21" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="T21" s="41">
         <v>105.271594851877</v>
       </c>
-      <c r="U21" s="34" t="s">
+      <c r="U21" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="V21" s="33"/>
-      <c r="W21" s="20">
-        <v>0.862131530155452</v>
-      </c>
-      <c r="X21" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="Y21" s="39">
-        <v>0.719304039555283</v>
-      </c>
-      <c r="Z21" s="32" t="s">
+      <c r="V21" s="28"/>
+      <c r="W21" s="16">
+        <v>0.86213153015545196</v>
+      </c>
+      <c r="X21" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y21" s="34">
+        <v>0.71930403955528299</v>
+      </c>
+      <c r="Z21" s="27" t="s">
         <v>47</v>
       </c>
       <c r="AA21" s="8"/>
@@ -5183,9 +4603,9 @@
       <c r="J24" s="8"/>
       <c r="K24" s="8"/>
       <c r="L24" s="8"/>
-      <c r="M24" s="44"/>
+      <c r="M24" s="39"/>
       <c r="N24" s="8"/>
-      <c r="O24" s="45"/>
+      <c r="O24" s="40"/>
       <c r="P24" s="7"/>
       <c r="Q24" s="7"/>
       <c r="R24" s="7"/>
@@ -5200,108 +4620,108 @@
       <c r="AA24" s="8"/>
       <c r="AB24" s="8"/>
     </row>
-    <row r="25" spans="3:6">
-      <c r="C25" s="9" t="s">
+    <row r="25" spans="1:28">
+      <c r="C25" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="21"/>
-    </row>
-    <row r="26" spans="3:13">
-      <c r="C26" s="11" t="s">
+      <c r="D25" s="52"/>
+      <c r="E25" s="52"/>
+      <c r="F25" s="53"/>
+    </row>
+    <row r="26" spans="1:28">
+      <c r="C26" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="23"/>
-      <c r="M26" s="28"/>
-    </row>
-    <row r="27" spans="3:13">
-      <c r="C27" s="13">
-        <v>0.132</v>
-      </c>
-      <c r="F27" s="35" t="s">
+      <c r="D26" s="55"/>
+      <c r="E26" s="55"/>
+      <c r="F26" s="56"/>
+      <c r="M26" s="23"/>
+    </row>
+    <row r="27" spans="1:28" ht="18">
+      <c r="C27" s="9">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="F27" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="G27" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="H27" s="25">
-        <v>0.0965063776002464</v>
-      </c>
-      <c r="M27" s="28"/>
-    </row>
-    <row r="28" spans="3:8">
-      <c r="C28" s="15">
-        <v>0.009</v>
-      </c>
-      <c r="F28" s="34" t="s">
+      <c r="G27" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="H27" s="20">
+        <v>9.6506377600246399E-2</v>
+      </c>
+      <c r="M27" s="23"/>
+    </row>
+    <row r="28" spans="1:28" ht="18">
+      <c r="C28" s="11">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="F28" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="G28" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="H28" s="26">
-        <v>0.0122558806800694</v>
-      </c>
-    </row>
-    <row r="29" spans="3:13">
-      <c r="C29" s="17">
+      <c r="G28" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="H28" s="21">
+        <v>1.22558806800694E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:28" ht="18">
+      <c r="C29" s="13">
         <v>0.996</v>
       </c>
-      <c r="F29" s="34" t="s">
+      <c r="F29" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="G29" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="H29" s="25">
-        <v>0.579582288921128</v>
-      </c>
-      <c r="M29" s="28"/>
-    </row>
-    <row r="30" spans="3:8">
-      <c r="C30" s="17">
-        <v>0.088</v>
-      </c>
-      <c r="F30" s="34" t="s">
+      <c r="G29" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="H29" s="20">
+        <v>0.57958228892112795</v>
+      </c>
+      <c r="M29" s="23"/>
+    </row>
+    <row r="30" spans="1:28" ht="18">
+      <c r="C30" s="13">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="F30" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="G30" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="H30" s="25">
-        <v>0.0657868338421766</v>
-      </c>
-    </row>
-    <row r="31" spans="3:13">
-      <c r="C31" s="17">
-        <v>1.787</v>
-      </c>
-      <c r="F31" s="34" t="s">
+      <c r="G30" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="H30" s="20">
+        <v>6.5786833842176595E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:28" ht="18">
+      <c r="C31" s="13">
+        <v>1.7869999999999999</v>
+      </c>
+      <c r="F31" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="G31" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="H31" s="25">
-        <v>1.84905922972114</v>
-      </c>
-      <c r="M31" s="28"/>
-    </row>
-    <row r="32" spans="3:8">
-      <c r="C32" s="15">
-        <v>0.007</v>
-      </c>
-      <c r="F32" s="34" t="s">
+      <c r="G31" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="H31" s="20">
+        <v>1.8490592297211399</v>
+      </c>
+      <c r="M31" s="23"/>
+    </row>
+    <row r="32" spans="1:28" ht="18">
+      <c r="C32" s="11">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="F32" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="G32" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="H32" s="26">
-        <v>0.00678518699644487</v>
+      <c r="G32" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="H32" s="21">
+        <v>6.7851869964448697E-3</v>
       </c>
     </row>
     <row r="33" spans="3:6">
@@ -5318,217 +4738,214 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="H2:K2"/>
-    <mergeCell ref="M2:P2"/>
-    <mergeCell ref="R2:U2"/>
-    <mergeCell ref="W2:Z2"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="M3:O3"/>
-    <mergeCell ref="R3:T3"/>
-    <mergeCell ref="W3:Y3"/>
+    <mergeCell ref="C25:F25"/>
+    <mergeCell ref="C26:F26"/>
     <mergeCell ref="C14:Z14"/>
     <mergeCell ref="C15:F15"/>
     <mergeCell ref="H15:K15"/>
     <mergeCell ref="M15:P15"/>
     <mergeCell ref="R15:U15"/>
     <mergeCell ref="W15:Z15"/>
-    <mergeCell ref="C25:F25"/>
-    <mergeCell ref="C26:F26"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="R3:T3"/>
+    <mergeCell ref="W3:Y3"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="H2:K2"/>
+    <mergeCell ref="M2:P2"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="W2:Z2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:F10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="B2:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F8" sqref="A1:F8"/>
+      <selection activeCell="B2" sqref="B2:G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.625" customWidth="true"/>
-    <col min="2" max="2" width="20.125" customWidth="true"/>
-    <col min="3" max="3" width="22.125" customWidth="true"/>
-    <col min="4" max="4" width="20.875" customWidth="true"/>
-    <col min="5" max="6" width="21.25" customWidth="true"/>
+    <col min="2" max="2" width="10.5703125" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" customWidth="1"/>
+    <col min="6" max="7" width="21.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
+    <row r="2" spans="2:7">
+      <c r="B2" s="1"/>
+      <c r="C2" s="57" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="1"/>
-      <c r="B2" s="3" t="s">
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
+    </row>
+    <row r="3" spans="2:7">
+      <c r="B3" s="1"/>
+      <c r="C3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="2:7" ht="18">
+      <c r="B4" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C4" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G4" s="4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="1" t="s">
+    <row r="5" spans="2:7" ht="18">
+      <c r="B5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="C5" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="F5" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="G5" s="5" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="1" t="s">
+    <row r="6" spans="2:7" ht="18">
+      <c r="B6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="C6" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="D6" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E6" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="F6" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="G6" s="4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="1" t="s">
+    <row r="7" spans="2:7" ht="18">
+      <c r="B7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="C7" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="D7" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="E7" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="F7" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="G7" s="4" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="1" t="s">
+    <row r="8" spans="2:7" ht="18">
+      <c r="B8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="C8" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="D8" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="E8" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="F8" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="G8" s="4" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="1" t="s">
+    <row r="9" spans="2:7" ht="18">
+      <c r="B9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="C9" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="D9" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="E9" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="F9" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="G9" s="4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
+    <row r="10" spans="2:7">
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+    </row>
+    <row r="11" spans="2:7">
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="C2:G2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>